<commit_message>
Resolve some old name confusion highlighted by fuzzy matching
</commit_message>
<xml_diff>
--- a/docs/xlsx/fuzzy_matching.xlsx
+++ b/docs/xlsx/fuzzy_matching.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mike\projects\work\wsw-results\docs\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D48B457-017F-412D-9E20-EE4C5A02B49B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44653BDA-D0F2-4C8E-B322-76A486ED2F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{11E0DFFD-4DF9-47BE-9F35-B0B5AD25860B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="105">
   <si>
     <t>'Alan Cross'</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t>No longer highlighted by fuzzy matching logic - due to Jon being a nickname for Jonathan</t>
+  </si>
+  <si>
+    <t>Different people - both competed simulataneously on 07/10/2008</t>
   </si>
 </sst>
 </file>
@@ -720,10 +723,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEB25BC-2D78-400D-806D-B9F8670BC859}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +751,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -762,7 +766,7 @@
         <v>('Alan Cross', 'Allan Cross'),</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
@@ -777,7 +781,7 @@
         <v>('Alex Bennett- Baggs', 'Alex Bennett-Baggs'),</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
@@ -792,7 +796,7 @@
         <v>('Alistair Williams', 'Alastair Williams'),</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>57</v>
       </c>
@@ -807,7 +811,7 @@
         <v>('Andy Harris', 'Andrew Harris'),</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -822,7 +826,7 @@
         <v>('Antony Baker', 'Anthony Baker'),</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>59</v>
       </c>
@@ -837,7 +841,7 @@
         <v>('Bjoern Haacke', 'Bjorn Haacke'),</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>60</v>
       </c>
@@ -852,7 +856,7 @@
         <v>('Charlie Wilson', 'Charles Wilson'),</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>61</v>
       </c>
@@ -867,7 +871,7 @@
         <v>('Claude Van Martin', 'Claude Van-Martyn'),</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>61</v>
       </c>
@@ -882,7 +886,7 @@
         <v>('Claude Van Martin', 'Claud Van Martin'),</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>62</v>
       </c>
@@ -897,7 +901,7 @@
         <v>('Claud Van Martin', 'Claude Van-Martyn'),</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>63</v>
       </c>
@@ -927,7 +931,7 @@
         <v>('Dave MacInnes', 'David MacInnes'),</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
@@ -972,7 +976,7 @@
         <v>('David Finch', 'Dave Finch'),</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>68</v>
       </c>
@@ -987,7 +991,7 @@
         <v>('Edward Murrell', 'Eddie Murrell'),</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>69</v>
       </c>
@@ -1002,7 +1006,7 @@
         <v>('Graham Holbert', 'Graham Hulbert'),</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>70</v>
       </c>
@@ -1017,7 +1021,7 @@
         <v>('Jim Paine', 'James Paine'),</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>71</v>
       </c>
@@ -1032,7 +1036,7 @@
         <v>('Joe Adams', 'Joseph Adams'),</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
@@ -1047,7 +1051,7 @@
         <v>('John Langdown', 'John Langdon'),</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>73</v>
       </c>
@@ -1080,7 +1084,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>75</v>
       </c>
@@ -1095,7 +1099,7 @@
         <v>('Malcom Barnsley', 'Malcolm Barnsley'),</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
@@ -1110,7 +1114,7 @@
         <v>('Mathew Spooner', 'Matthew Spooner'),</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>77</v>
       </c>
@@ -1125,7 +1129,7 @@
         <v>('Matthew Burridge', 'Mathew Burridge'),</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>78</v>
       </c>
@@ -1140,7 +1144,7 @@
         <v>('Matthew Philpott', 'Matt Philpott'),</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>79</v>
       </c>
@@ -1155,7 +1159,7 @@
         <v>('Michael Walklin', 'Mike Walklin'),</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>80</v>
       </c>
@@ -1185,7 +1189,7 @@
         <v>('Nills Haarbosch', 'Neils Haarbosch'),</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>82</v>
       </c>
@@ -1200,7 +1204,7 @@
         <v>('Pete Cunningham', 'Peter Cunningham'),</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>83</v>
       </c>
@@ -1215,7 +1219,7 @@
         <v>('Pete Martin', 'Peter Martin'),</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>84</v>
       </c>
@@ -1230,7 +1234,7 @@
         <v>('Peter Davis', 'Pete Davis'),</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>85</v>
       </c>
@@ -1245,7 +1249,7 @@
         <v>('Peter Young', 'Pete Young'),</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>86</v>
       </c>
@@ -1260,7 +1264,7 @@
         <v>('Phil Lewin', 'Philip Lewin'),</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>87</v>
       </c>
@@ -1275,7 +1279,7 @@
         <v>('Piere Saville', 'Pierre Saville'),</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>88</v>
       </c>
@@ -1290,7 +1294,7 @@
         <v>('Robert Date', 'Bob Date'),</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>89</v>
       </c>
@@ -1305,7 +1309,7 @@
         <v>('Robert Spagnoletti', 'Bob Spagnoletti'),</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>90</v>
       </c>
@@ -1338,7 +1342,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>92</v>
       </c>
@@ -1354,18 +1358,21 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="4" t="s">
         <v>53</v>
       </c>
       <c r="E42" s="3" t="str">
         <f t="shared" si="0"/>
         <v>('Simon Perks', 'Simon Perkins'),</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
@@ -1383,7 +1390,7 @@
         <v>('Stephen Davison', 'Steve Davidson'),</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>94</v>
       </c>
@@ -1428,7 +1435,7 @@
         <v>('Steven Summerfield', 'Steve Summerfield'),</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>97</v>
       </c>
@@ -1473,7 +1480,7 @@
         <v>('Will Oscroft', 'William Oscroft'),</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>100</v>
       </c>
@@ -1488,7 +1495,7 @@
         <v>('Will Trossell', 'William Trossell'),</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>101</v>
       </c>
@@ -1504,7 +1511,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C51" xr:uid="{FDEB25BC-2D78-400D-806D-B9F8670BC859}"/>
+  <autoFilter ref="A1:C51" xr:uid="{FDEB25BC-2D78-400D-806D-B9F8670BC859}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="N"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update fuzzy matching notes
</commit_message>
<xml_diff>
--- a/docs/xlsx/fuzzy_matching.xlsx
+++ b/docs/xlsx/fuzzy_matching.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\mike\projects\work\wsw-results\docs\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44653BDA-D0F2-4C8E-B322-76A486ED2F55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC765B3-F164-45D6-8E42-0D5B0F337A21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{11E0DFFD-4DF9-47BE-9F35-B0B5AD25860B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="106">
   <si>
     <t>'Alan Cross'</t>
   </si>
@@ -350,6 +350,9 @@
   </si>
   <si>
     <t>Different people - both competed simulataneously on 07/10/2008</t>
+  </si>
+  <si>
+    <t>TODO</t>
   </si>
 </sst>
 </file>
@@ -723,11 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDEB25BC-2D78-400D-806D-B9F8670BC859}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,7 +753,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -766,7 +768,7 @@
         <v>('Alan Cross', 'Allan Cross'),</v>
       </c>
     </row>
-    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
@@ -781,7 +783,7 @@
         <v>('Alex Bennett- Baggs', 'Alex Bennett-Baggs'),</v>
       </c>
     </row>
-    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>56</v>
       </c>
@@ -796,7 +798,7 @@
         <v>('Alistair Williams', 'Alastair Williams'),</v>
       </c>
     </row>
-    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>57</v>
       </c>
@@ -811,7 +813,7 @@
         <v>('Andy Harris', 'Andrew Harris'),</v>
       </c>
     </row>
-    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>58</v>
       </c>
@@ -826,7 +828,7 @@
         <v>('Antony Baker', 'Anthony Baker'),</v>
       </c>
     </row>
-    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>59</v>
       </c>
@@ -841,7 +843,7 @@
         <v>('Bjoern Haacke', 'Bjorn Haacke'),</v>
       </c>
     </row>
-    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>60</v>
       </c>
@@ -856,7 +858,7 @@
         <v>('Charlie Wilson', 'Charles Wilson'),</v>
       </c>
     </row>
-    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>61</v>
       </c>
@@ -871,7 +873,7 @@
         <v>('Claude Van Martin', 'Claude Van-Martyn'),</v>
       </c>
     </row>
-    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>61</v>
       </c>
@@ -886,7 +888,7 @@
         <v>('Claude Van Martin', 'Claud Van Martin'),</v>
       </c>
     </row>
-    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>62</v>
       </c>
@@ -901,7 +903,7 @@
         <v>('Claud Van Martin', 'Claude Van-Martyn'),</v>
       </c>
     </row>
-    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>63</v>
       </c>
@@ -917,13 +919,13 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E13" s="3" t="str">
@@ -931,7 +933,7 @@
         <v>('Dave MacInnes', 'David MacInnes'),</v>
       </c>
     </row>
-    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>65</v>
       </c>
@@ -947,13 +949,13 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E15" s="3" t="str">
@@ -962,13 +964,13 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E16" s="3" t="str">
@@ -976,7 +978,7 @@
         <v>('David Finch', 'Dave Finch'),</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>68</v>
       </c>
@@ -991,7 +993,7 @@
         <v>('Edward Murrell', 'Eddie Murrell'),</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>69</v>
       </c>
@@ -1006,7 +1008,7 @@
         <v>('Graham Holbert', 'Graham Hulbert'),</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>70</v>
       </c>
@@ -1021,7 +1023,7 @@
         <v>('Jim Paine', 'James Paine'),</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>71</v>
       </c>
@@ -1036,7 +1038,7 @@
         <v>('Joe Adams', 'Joseph Adams'),</v>
       </c>
     </row>
-    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>72</v>
       </c>
@@ -1051,7 +1053,7 @@
         <v>('John Langdown', 'John Langdon'),</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>73</v>
       </c>
@@ -1084,7 +1086,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>75</v>
       </c>
@@ -1099,7 +1101,7 @@
         <v>('Malcom Barnsley', 'Malcolm Barnsley'),</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>76</v>
       </c>
@@ -1114,7 +1116,7 @@
         <v>('Mathew Spooner', 'Matthew Spooner'),</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>77</v>
       </c>
@@ -1129,7 +1131,7 @@
         <v>('Matthew Burridge', 'Mathew Burridge'),</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>78</v>
       </c>
@@ -1144,7 +1146,7 @@
         <v>('Matthew Philpott', 'Matt Philpott'),</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>79</v>
       </c>
@@ -1159,7 +1161,7 @@
         <v>('Michael Walklin', 'Mike Walklin'),</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>80</v>
       </c>
@@ -1188,8 +1190,11 @@
         <f t="shared" si="0"/>
         <v>('Nills Haarbosch', 'Neils Haarbosch'),</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="J30" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>82</v>
       </c>
@@ -1204,7 +1209,7 @@
         <v>('Pete Cunningham', 'Peter Cunningham'),</v>
       </c>
     </row>
-    <row r="32" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>83</v>
       </c>
@@ -1219,7 +1224,7 @@
         <v>('Pete Martin', 'Peter Martin'),</v>
       </c>
     </row>
-    <row r="33" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>84</v>
       </c>
@@ -1234,7 +1239,7 @@
         <v>('Peter Davis', 'Pete Davis'),</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>85</v>
       </c>
@@ -1249,7 +1254,7 @@
         <v>('Peter Young', 'Pete Young'),</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>86</v>
       </c>
@@ -1264,7 +1269,7 @@
         <v>('Phil Lewin', 'Philip Lewin'),</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>87</v>
       </c>
@@ -1279,7 +1284,7 @@
         <v>('Piere Saville', 'Pierre Saville'),</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>88</v>
       </c>
@@ -1294,7 +1299,7 @@
         <v>('Robert Date', 'Bob Date'),</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>89</v>
       </c>
@@ -1309,7 +1314,7 @@
         <v>('Robert Spagnoletti', 'Bob Spagnoletti'),</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>90</v>
       </c>
@@ -1342,7 +1347,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>92</v>
       </c>
@@ -1376,13 +1381,13 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E43" s="3" t="str">
@@ -1390,7 +1395,7 @@
         <v>('Stephen Davison', 'Steve Davidson'),</v>
       </c>
     </row>
-    <row r="44" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>94</v>
       </c>
@@ -1406,13 +1411,13 @@
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E45" s="3" t="str">
@@ -1421,13 +1426,13 @@
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E46" s="3" t="str">
@@ -1435,7 +1440,7 @@
         <v>('Steven Summerfield', 'Steve Summerfield'),</v>
       </c>
     </row>
-    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>97</v>
       </c>
@@ -1451,13 +1456,13 @@
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E48" s="3" t="str">
@@ -1466,13 +1471,13 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="1" t="s">
         <v>53</v>
       </c>
       <c r="E49" s="3" t="str">
@@ -1480,7 +1485,7 @@
         <v>('Will Oscroft', 'William Oscroft'),</v>
       </c>
     </row>
-    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>100</v>
       </c>
@@ -1495,7 +1500,7 @@
         <v>('Will Trossell', 'William Trossell'),</v>
       </c>
     </row>
-    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>101</v>
       </c>
@@ -1511,13 +1516,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C51" xr:uid="{FDEB25BC-2D78-400D-806D-B9F8670BC859}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="N"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C51" xr:uid="{FDEB25BC-2D78-400D-806D-B9F8670BC859}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>